<commit_message>
Subiendo script y cambios de Api v3
</commit_message>
<xml_diff>
--- a/Excel/TablasTablas.xlsx
+++ b/Excel/TablasTablas.xlsx
@@ -1,61 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabajo\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13199513-1362-432C-B286-146BFF89897D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E6467B-3AAE-4170-A811-E2C759A5B3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{720E2F46-AD94-4C2A-9926-903B16614509}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{720E2F46-AD94-4C2A-9926-903B16614509}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>IdTabla</t>
-  </si>
-  <si>
-    <t>NombreTabla</t>
-  </si>
-  <si>
-    <t>IdCampo</t>
-  </si>
-  <si>
     <t>Valor</t>
   </si>
   <si>
-    <t>TablaTablas</t>
-  </si>
-  <si>
     <t>Centro Juvenil</t>
   </si>
   <si>
@@ -95,12 +72,6 @@
     <t>NivelRiesgo</t>
   </si>
   <si>
-    <t>Indicadores</t>
-  </si>
-  <si>
-    <t>NombreIndicador</t>
-  </si>
-  <si>
     <t>Indicador 1</t>
   </si>
   <si>
@@ -186,13 +157,34 @@
   </si>
   <si>
     <t>Indicador 26</t>
+  </si>
+  <si>
+    <t>TableTables</t>
+  </si>
+  <si>
+    <t>idindicator</t>
+  </si>
+  <si>
+    <t>nametable</t>
+  </si>
+  <si>
+    <t>idfield</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>nameindicator</t>
+  </si>
+  <si>
+    <t>Indicator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,67 +637,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA50205-7B3A-4C07-8150-05548D1E474D}">
   <dimension ref="D3:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.09765625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:18">
       <c r="F3" s="6" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="4:18" ht="18" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="4:18" ht="17.399999999999999">
       <c r="D6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="4:18" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="4:18">
       <c r="D7" s="1">
         <v>1</v>
       </c>
@@ -713,19 +705,19 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="O7" s="1">
         <v>1</v>
@@ -740,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:18">
       <c r="D8" s="1">
         <v>2</v>
       </c>
@@ -748,19 +740,19 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3">
         <v>2</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K8" s="1">
         <v>2</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="O8" s="1">
         <v>2</v>
@@ -775,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:18">
       <c r="D9" s="1">
         <v>3</v>
       </c>
@@ -783,19 +775,19 @@
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G9" s="3">
         <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K9" s="1">
         <v>3</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="O9" s="1">
         <v>3</v>
@@ -810,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:18">
       <c r="D10" s="1">
         <v>4</v>
       </c>
@@ -818,19 +810,19 @@
         <v>2</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K10" s="1">
         <v>4</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O10" s="1">
         <v>4</v>
@@ -845,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:18">
       <c r="D11" s="1">
         <v>5</v>
       </c>
@@ -853,19 +845,19 @@
         <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K11" s="1">
         <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="O11" s="1">
         <v>5</v>
@@ -880,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:18">
       <c r="D12" s="1">
         <v>6</v>
       </c>
@@ -888,19 +880,19 @@
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G12" s="4">
         <v>3</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K12" s="1">
         <v>6</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O12" s="1">
         <v>6</v>
@@ -915,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:18">
       <c r="D13" s="1">
         <v>7</v>
       </c>
@@ -923,19 +915,19 @@
         <v>3</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G13" s="5">
         <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K13" s="1">
         <v>7</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="O13" s="1">
         <v>7</v>
@@ -950,7 +942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:18">
       <c r="D14" s="1">
         <v>8</v>
       </c>
@@ -958,19 +950,19 @@
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G14" s="5">
         <v>2</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K14" s="1">
         <v>8</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O14" s="1">
         <v>8</v>
@@ -985,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:18">
       <c r="D15" s="1">
         <v>9</v>
       </c>
@@ -993,19 +985,19 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G15" s="5">
         <v>3</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K15" s="1">
         <v>9</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O15" s="1">
         <v>9</v>
@@ -1014,7 +1006,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:18">
       <c r="D16" s="1">
         <v>10</v>
       </c>
@@ -1022,19 +1014,19 @@
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G16" s="5">
         <v>4</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="K16" s="1">
         <v>10</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="O16" s="1">
         <v>10</v>
@@ -1043,7 +1035,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:18">
       <c r="D17" s="1">
         <v>11</v>
       </c>
@@ -1055,7 +1047,7 @@
         <v>11</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="O17" s="1">
         <v>11</v>
@@ -1064,7 +1056,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:18">
       <c r="D18" s="1">
         <v>12</v>
       </c>
@@ -1076,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="O18" s="1">
         <v>12</v>
@@ -1085,7 +1077,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:18">
       <c r="D19" s="1">
         <v>13</v>
       </c>
@@ -1097,7 +1089,7 @@
         <v>13</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="O19" s="1">
         <v>13</v>
@@ -1106,7 +1098,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:18">
       <c r="D20" s="1">
         <v>14</v>
       </c>
@@ -1118,7 +1110,7 @@
         <v>14</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="O20" s="1">
         <v>14</v>
@@ -1127,7 +1119,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:18">
       <c r="D21" s="1">
         <v>15</v>
       </c>
@@ -1139,7 +1131,7 @@
         <v>15</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="O21" s="1">
         <v>15</v>
@@ -1148,7 +1140,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:18">
       <c r="D22" s="1">
         <v>16</v>
       </c>
@@ -1160,7 +1152,7 @@
         <v>16</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O22" s="1">
         <v>16</v>
@@ -1169,7 +1161,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:18">
       <c r="D23" s="1">
         <v>17</v>
       </c>
@@ -1181,7 +1173,7 @@
         <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="O23" s="1">
         <v>17</v>
@@ -1190,7 +1182,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:18">
       <c r="D24" s="1">
         <v>18</v>
       </c>
@@ -1202,7 +1194,7 @@
         <v>18</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O24" s="1">
         <v>18</v>
@@ -1211,7 +1203,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:18">
       <c r="D25" s="1">
         <v>19</v>
       </c>
@@ -1223,7 +1215,7 @@
         <v>19</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O25" s="1">
         <v>19</v>
@@ -1232,7 +1224,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:18">
       <c r="D26" s="1">
         <v>20</v>
       </c>
@@ -1244,7 +1236,7 @@
         <v>20</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="O26" s="1">
         <v>20</v>
@@ -1253,7 +1245,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:18">
       <c r="D27" s="1">
         <v>21</v>
       </c>
@@ -1265,7 +1257,7 @@
         <v>21</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="O27" s="1">
         <v>21</v>
@@ -1274,7 +1266,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:18">
       <c r="D28" s="1">
         <v>22</v>
       </c>
@@ -1286,7 +1278,7 @@
         <v>22</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O28" s="1">
         <v>22</v>
@@ -1295,7 +1287,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:18">
       <c r="D29" s="1">
         <v>23</v>
       </c>
@@ -1307,7 +1299,7 @@
         <v>23</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O29" s="1">
         <v>23</v>
@@ -1316,7 +1308,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:18">
       <c r="D30" s="1">
         <v>24</v>
       </c>
@@ -1328,7 +1320,7 @@
         <v>24</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="O30" s="1">
         <v>24</v>
@@ -1337,7 +1329,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:18">
       <c r="D31" s="1">
         <v>25</v>
       </c>
@@ -1349,7 +1341,7 @@
         <v>25</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O31" s="1">
         <v>25</v>
@@ -1358,12 +1350,12 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:18">
       <c r="K32" s="10">
         <v>26</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="O32" s="1">
         <v>26</v>

</xml_diff>

<commit_message>
Añadiendo aplicación móvil prototipo
</commit_message>
<xml_diff>
--- a/Excel/TablasTablas.xlsx
+++ b/Excel/TablasTablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabajo\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E6467B-3AAE-4170-A811-E2C759A5B3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACA22EE-4F28-42F8-9821-2898568CB4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{720E2F46-AD94-4C2A-9926-903B16614509}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{720E2F46-AD94-4C2A-9926-903B16614509}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Valor</t>
-  </si>
-  <si>
     <t>Centro Juvenil</t>
   </si>
   <si>
@@ -147,12 +144,6 @@
     <t>Indicador 25</t>
   </si>
   <si>
-    <t>IndicadorID</t>
-  </si>
-  <si>
-    <t>ProcesoID</t>
-  </si>
-  <si>
     <t>Valores Indicadores(Sábana)</t>
   </si>
   <si>
@@ -178,6 +169,30 @@
   </si>
   <si>
     <t>Indicator</t>
+  </si>
+  <si>
+    <t>FK de Indicator</t>
+  </si>
+  <si>
+    <t>indicadorid</t>
+  </si>
+  <si>
+    <t>processid</t>
+  </si>
+  <si>
+    <t>Ayacucho</t>
+  </si>
+  <si>
+    <t>FK = TableTables</t>
+  </si>
+  <si>
+    <t>campo para mapear el tipo de proceso al que pertenece una sabana</t>
+  </si>
+  <si>
+    <t>TablaProcesoPendiente</t>
+  </si>
+  <si>
+    <t>A partir de esta tabla se armarán las gráficas</t>
   </si>
 </sst>
 </file>
@@ -289,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -301,6 +316,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,159 +665,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA50205-7B3A-4C07-8150-05548D1E474D}">
-  <dimension ref="D3:R32"/>
+  <dimension ref="D1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:L11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
+    <col min="5" max="5" width="15.19921875" customWidth="1"/>
     <col min="6" max="6" width="15.296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.09765625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.59765625" customWidth="1"/>
     <col min="18" max="18" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:18">
+    <row r="1" spans="4:23">
+      <c r="O1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+    </row>
+    <row r="3" spans="4:23">
       <c r="F3" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="4:18" ht="17.399999999999999">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="4:23">
+      <c r="R4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+    </row>
+    <row r="5" spans="4:23">
+      <c r="E5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+    </row>
+    <row r="6" spans="4:23" ht="17.399999999999999">
       <c r="D6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="4:18">
+        <v>50</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="4:23">
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="11">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:23">
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="1">
-        <v>1</v>
-      </c>
-      <c r="P7" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>20</v>
-      </c>
-      <c r="R7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="4:18">
-      <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="1">
-        <v>2</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="O8" s="1">
         <v>2</v>
       </c>
       <c r="P8" s="1">
         <v>2</v>
       </c>
-      <c r="Q8" s="1">
-        <v>30</v>
+      <c r="Q8" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:18">
+    <row r="9" spans="4:23">
       <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="11">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K9" s="1">
         <v>3</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O9" s="1">
         <v>3</v>
@@ -795,34 +859,34 @@
       <c r="P9" s="1">
         <v>3</v>
       </c>
-      <c r="Q9" s="1">
-        <v>40</v>
+      <c r="Q9" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R9" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:18">
+    <row r="10" spans="4:23">
       <c r="D10" s="1">
         <v>4</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="12">
         <v>2</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="K10" s="1">
         <v>4</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O10" s="1">
         <v>4</v>
@@ -830,34 +894,34 @@
       <c r="P10" s="8">
         <v>4</v>
       </c>
-      <c r="Q10" s="1">
-        <v>50</v>
+      <c r="Q10" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R10" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:18">
+    <row r="11" spans="4:23">
       <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="12">
         <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" s="1">
         <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O11" s="1">
         <v>5</v>
@@ -865,34 +929,34 @@
       <c r="P11" s="1">
         <v>1</v>
       </c>
-      <c r="Q11" s="1">
-        <v>10</v>
+      <c r="Q11" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R11" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:18">
+    <row r="12" spans="4:23">
       <c r="D12" s="1">
         <v>6</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="12">
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" s="4">
         <v>3</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K12" s="1">
         <v>6</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O12" s="1">
         <v>6</v>
@@ -900,34 +964,34 @@
       <c r="P12" s="1">
         <v>2</v>
       </c>
-      <c r="Q12" s="1">
-        <v>25</v>
+      <c r="Q12" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R12" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="4:18">
+    <row r="13" spans="4:23">
       <c r="D13" s="1">
         <v>7</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="13">
         <v>3</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="5">
         <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K13" s="1">
         <v>7</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O13" s="1">
         <v>7</v>
@@ -935,34 +999,34 @@
       <c r="P13" s="9">
         <v>3</v>
       </c>
-      <c r="Q13" s="1">
-        <v>30</v>
+      <c r="Q13" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R13" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="4:18">
+    <row r="14" spans="4:23">
       <c r="D14" s="1">
         <v>8</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="13">
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="5">
         <v>2</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K14" s="1">
         <v>8</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O14" s="1">
         <v>8</v>
@@ -970,34 +1034,34 @@
       <c r="P14" s="1">
         <v>4</v>
       </c>
-      <c r="Q14" s="1">
-        <v>40</v>
+      <c r="Q14" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R14" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:18">
+    <row r="15" spans="4:23">
       <c r="D15" s="1">
         <v>9</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="13">
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="5">
         <v>3</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K15" s="1">
         <v>9</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O15" s="1">
         <v>9</v>
@@ -1006,27 +1070,27 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="4:18">
+    <row r="16" spans="4:23">
       <c r="D16" s="1">
         <v>10</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="13">
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" s="5">
         <v>4</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K16" s="1">
         <v>10</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O16" s="1">
         <v>10</v>
@@ -1047,7 +1111,7 @@
         <v>11</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O17" s="1">
         <v>11</v>
@@ -1068,7 +1132,7 @@
         <v>12</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O18" s="1">
         <v>12</v>
@@ -1089,7 +1153,7 @@
         <v>13</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O19" s="1">
         <v>13</v>
@@ -1110,7 +1174,7 @@
         <v>14</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O20" s="1">
         <v>14</v>
@@ -1131,7 +1195,7 @@
         <v>15</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O21" s="1">
         <v>15</v>
@@ -1152,7 +1216,7 @@
         <v>16</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O22" s="1">
         <v>16</v>
@@ -1173,7 +1237,7 @@
         <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O23" s="1">
         <v>17</v>
@@ -1194,7 +1258,7 @@
         <v>18</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O24" s="1">
         <v>18</v>
@@ -1215,7 +1279,7 @@
         <v>19</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O25" s="1">
         <v>19</v>
@@ -1236,7 +1300,7 @@
         <v>20</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O26" s="1">
         <v>20</v>
@@ -1257,7 +1321,7 @@
         <v>21</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O27" s="1">
         <v>21</v>
@@ -1278,7 +1342,7 @@
         <v>22</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O28" s="1">
         <v>22</v>
@@ -1299,7 +1363,7 @@
         <v>23</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O29" s="1">
         <v>23</v>
@@ -1320,7 +1384,7 @@
         <v>24</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O30" s="1">
         <v>24</v>
@@ -1341,7 +1405,7 @@
         <v>25</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O31" s="1">
         <v>25</v>
@@ -1355,7 +1419,7 @@
         <v>26</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O32" s="1">
         <v>26</v>
@@ -1365,6 +1429,10 @@
       <c r="R32" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="R4:U5"/>
+    <mergeCell ref="O1:R1"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>